<commit_message>
Finished database, added low-level search function
</commit_message>
<xml_diff>
--- a/backend/app/data/Dauphiné.xlsx
+++ b/backend/app/data/Dauphiné.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alyssa/Documents/GitHub/playing-cards/backend/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4F86CD-3447-CC46-BEA3-C5F46D4E1C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703F3347-E711-6646-BC72-00AF6A32459E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7140" yWindow="500" windowWidth="21660" windowHeight="16340" xr2:uid="{CE2FDC2A-7548-B946-A288-0CC89512212C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="48">
   <si>
     <t>Card</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Start Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Cartes de tête issues de jeux au portrait du Dauphiné</t>
   </si>
 </sst>
 </file>
@@ -548,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12460001-25AC-2F48-B939-A0BEC1246E5F}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +566,7 @@
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -574,28 +580,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -608,26 +617,29 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>1746</v>
+      <c r="E2" t="s">
+        <v>47</v>
       </c>
       <c r="F2">
-        <v>1777</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G2">
+        <v>1777</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -640,26 +652,29 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>1746</v>
+      <c r="E3" t="s">
+        <v>47</v>
       </c>
       <c r="F3">
-        <v>1777</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G3">
+        <v>1777</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -672,26 +687,29 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
-        <v>1746</v>
+      <c r="E4" t="s">
+        <v>47</v>
       </c>
       <c r="F4">
-        <v>1777</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G4">
+        <v>1777</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -704,26 +722,29 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
-        <v>1746</v>
+      <c r="E5" t="s">
+        <v>47</v>
       </c>
       <c r="F5">
-        <v>1777</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G5">
+        <v>1777</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -736,26 +757,29 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
-        <v>1746</v>
+      <c r="E6" t="s">
+        <v>47</v>
       </c>
       <c r="F6">
-        <v>1777</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G6">
+        <v>1777</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -768,26 +792,29 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>1746</v>
+      <c r="E7" t="s">
+        <v>47</v>
       </c>
       <c r="F7">
-        <v>1777</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G7">
+        <v>1777</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -800,26 +827,29 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
-        <v>1746</v>
+      <c r="E8" t="s">
+        <v>47</v>
       </c>
       <c r="F8">
-        <v>1777</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G8">
+        <v>1777</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -832,26 +862,29 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9">
-        <v>1746</v>
+      <c r="E9" t="s">
+        <v>47</v>
       </c>
       <c r="F9">
-        <v>1777</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G9">
+        <v>1777</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -864,26 +897,29 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10">
-        <v>1746</v>
+      <c r="E10" t="s">
+        <v>47</v>
       </c>
       <c r="F10">
-        <v>1777</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G10">
+        <v>1777</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -896,26 +932,29 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11">
-        <v>1746</v>
+      <c r="E11" t="s">
+        <v>47</v>
       </c>
       <c r="F11">
-        <v>1777</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G11">
+        <v>1777</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -928,26 +967,29 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12">
-        <v>1746</v>
+      <c r="E12" t="s">
+        <v>47</v>
       </c>
       <c r="F12">
-        <v>1777</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G12">
+        <v>1777</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -960,26 +1002,29 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13">
-        <v>1746</v>
+      <c r="E13" t="s">
+        <v>47</v>
       </c>
       <c r="F13">
-        <v>1777</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G13">
+        <v>1777</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -992,26 +1037,29 @@
       <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E14">
-        <v>1746</v>
+      <c r="E14" t="s">
+        <v>47</v>
       </c>
       <c r="F14">
-        <v>1777</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G14">
+        <v>1777</v>
       </c>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1024,26 +1072,29 @@
       <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="E15">
-        <v>1746</v>
+      <c r="E15" t="s">
+        <v>47</v>
       </c>
       <c r="F15">
-        <v>1777</v>
-      </c>
-      <c r="G15" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G15">
+        <v>1777</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1056,26 +1107,29 @@
       <c r="D16" t="s">
         <v>11</v>
       </c>
-      <c r="E16">
-        <v>1746</v>
+      <c r="E16" t="s">
+        <v>47</v>
       </c>
       <c r="F16">
-        <v>1777</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G16">
+        <v>1777</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1088,26 +1142,29 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
-      <c r="E17">
-        <v>1746</v>
+      <c r="E17" t="s">
+        <v>47</v>
       </c>
       <c r="F17">
-        <v>1777</v>
-      </c>
-      <c r="G17" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G17">
+        <v>1777</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1120,26 +1177,29 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E18">
-        <v>1746</v>
+      <c r="E18" t="s">
+        <v>47</v>
       </c>
       <c r="F18">
-        <v>1777</v>
-      </c>
-      <c r="G18" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G18">
+        <v>1777</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1152,26 +1212,29 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-      <c r="E19">
-        <v>1746</v>
+      <c r="E19" t="s">
+        <v>47</v>
       </c>
       <c r="F19">
-        <v>1777</v>
-      </c>
-      <c r="G19" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G19">
+        <v>1777</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1184,26 +1247,29 @@
       <c r="D20" t="s">
         <v>14</v>
       </c>
-      <c r="E20">
-        <v>1746</v>
+      <c r="E20" t="s">
+        <v>47</v>
       </c>
       <c r="F20">
-        <v>1777</v>
-      </c>
-      <c r="G20" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G20">
+        <v>1777</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1216,26 +1282,29 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
-        <v>1746</v>
+      <c r="E21" t="s">
+        <v>47</v>
       </c>
       <c r="F21">
-        <v>1777</v>
-      </c>
-      <c r="G21" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G21">
+        <v>1777</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1248,26 +1317,29 @@
       <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="E22">
-        <v>1746</v>
+      <c r="E22" t="s">
+        <v>47</v>
       </c>
       <c r="F22">
-        <v>1777</v>
-      </c>
-      <c r="G22" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G22">
+        <v>1777</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1280,27 +1352,30 @@
       <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E23">
-        <v>1746</v>
+      <c r="E23" t="s">
+        <v>47</v>
       </c>
       <c r="F23">
-        <v>1777</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
+        <v>1746</v>
+      </c>
+      <c r="G23">
+        <v>1777</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I23" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K24" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>